<commit_message>
Consolidate Extracted Excel Files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\Documents\UiPath\UiPathDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7B00AF-2178-4736-82B5-37DB08E53D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6A9428-9560-4A23-A856-6A739D4FF4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -180,10 +180,46 @@
     <t>Input_PaySlip_Path</t>
   </si>
   <si>
-    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Input</t>
-  </si>
-  <si>
     <t>tTAcUxfFUNKCBZK0c3lR9uvC+I4YWjy+y3Zqo7Fx2nGl1ws+vx52qcQbgsFUjrt5lQRLqANPznFvdl84Qbq6OQ==</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Output\Consolidated Excel\</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Output\Processed\</t>
+  </si>
+  <si>
+    <t>Conolidated_Excel_Path</t>
+  </si>
+  <si>
+    <t>Processed_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Input\</t>
+  </si>
+  <si>
+    <t>Output_Excel_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Output\</t>
+  </si>
+  <si>
+    <t>Output_Sheet_Name</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Update_Excel_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Output\Updated Excel\</t>
+  </si>
+  <si>
+    <t>Salary_Prediction_URL</t>
+  </si>
+  <si>
+    <t>https://rpa-demo-api.herokuapp.com/</t>
   </si>
 </sst>
 </file>
@@ -603,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +734,7 @@
         <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -706,7 +742,55 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Action Center Validation Added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\Documents\UiPath\UiPathDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BE8D22-3EE6-403E-B8EC-628AD602C9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C6B60-40CD-462F-8744-F11B654D1F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Excel_Employee_Path</t>
+  </si>
+  <si>
+    <t>Processed_PaySlip_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\Documents\UiPath\UiPathDemo\Input\Processed\</t>
   </si>
 </sst>
 </file>
@@ -645,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,59 +757,67 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>53</v>
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>